<commit_message>
exe-file, uml, docstrings fehlen noch
</commit_message>
<xml_diff>
--- a/zoo3aktiv/orgarnisatorisch/Checkliste aktuell.xlsx
+++ b/zoo3aktiv/orgarnisatorisch/Checkliste aktuell.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Umschueler\AppData\Roaming\Python\Python311\pyprojects\PycharmProjects\objektorientiert\git_project\zoo3aktiv\test\zoonew\zoo3aktiv\orgarnisatorisch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F91C524-BD8E-4988-9041-A26D25D667C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5CDE29D-AF94-46FA-923C-7F33D326F85B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6D91939B-A5B5-4F9B-AB36-190C3727F6FB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="49">
   <si>
     <t>Checkliste</t>
   </si>
@@ -213,7 +213,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -262,6 +262,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="21">
     <border>
@@ -495,7 +501,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -575,6 +581,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -590,16 +605,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -919,7 +928,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -932,10 +941,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="33"/>
+      <c r="B1" s="36"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -943,16 +952,16 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="37"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="40"/>
     </row>
     <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="12"/>
@@ -989,7 +998,7 @@
       <c r="D4" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="41"/>
+      <c r="E4" s="35"/>
       <c r="F4" s="28">
         <v>45319</v>
       </c>
@@ -1121,7 +1130,7 @@
       <c r="D10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="39"/>
+      <c r="E10" s="33"/>
       <c r="F10" s="24">
         <v>45319</v>
       </c>
@@ -1141,7 +1150,7 @@
       <c r="D11" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="40"/>
+      <c r="E11" s="34"/>
       <c r="F11" s="24">
         <v>45319</v>
       </c>
@@ -1181,7 +1190,7 @@
       <c r="D13" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="21"/>
+      <c r="E13" s="41"/>
       <c r="F13" s="24">
         <v>45319</v>
       </c>
@@ -1219,19 +1228,21 @@
       <c r="B15" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="6"/>
+      <c r="C15" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="D15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="38"/>
+      <c r="E15" s="7"/>
       <c r="F15" s="24">
         <v>45319</v>
       </c>
-      <c r="G15" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="H15" s="9">
-        <v>45321</v>
+      <c r="G15" s="19">
+        <v>100</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -1267,7 +1278,7 @@
       <c r="D17" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="39"/>
+      <c r="E17" s="33"/>
       <c r="F17" s="24">
         <v>45319</v>
       </c>
@@ -1283,11 +1294,11 @@
       <c r="B18" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="6"/>
+      <c r="C18" s="42"/>
       <c r="D18" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="21"/>
+      <c r="E18" s="41"/>
       <c r="F18" s="24">
         <v>45319</v>
       </c>
@@ -1371,7 +1382,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="G5 G11:G12 G14:G16 G19:G20" numberStoredAsText="1"/>
+    <ignoredError sqref="G5 G11:G12 G14 G19:G20 G16" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>